<commit_message>
Remove duplicates, convert to xlsx and clear custom styles
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_CCS.xlsx
+++ b/SuppXLS/Scen_ELC_CCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA2\Veda_models\I3p0_ELC_12TS_1REG_2020.08.15\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7B73C5-69A8-41C0-BD37-6C3FF89E1F69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995F9822-2F1B-402F-B001-8832266C85E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UC_CCS" sheetId="1" r:id="rId1"/>
@@ -169,11 +169,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -191,7 +191,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -206,12 +206,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -289,28 +283,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -320,10 +312,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 26" xfId="1" xr:uid="{355D50B4-CF94-4F2C-A124-50055F1831AE}"/>
-    <cellStyle name="Normale_Scen_UC_IND-StrucConst" xfId="2" xr:uid="{E39333DE-891B-4DB0-A94A-E451B8D3B2C9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -601,15 +591,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +614,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -655,7 +646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="7" t="s">
@@ -679,7 +670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="9" t="s">
@@ -703,7 +694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="7" t="s">
@@ -727,7 +718,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="7" t="s">
@@ -751,7 +742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="9" t="s">
@@ -775,7 +766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
@@ -799,27 +790,27 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="B12" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="E14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="B15" s="14" t="s">
         <v>22</v>
       </c>
@@ -845,7 +836,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -868,7 +859,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9">
       <c r="B17" t="s">
         <v>30</v>
       </c>
@@ -891,7 +882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -914,7 +905,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9">
       <c r="B19" t="s">
         <v>34</v>
       </c>
@@ -937,7 +928,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Adjusted to Naming Convention
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_CCS.xlsx
+++ b/SuppXLS/Scen_ELC_CCS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\I3p0_ELC_12TS_1REG_2020.11.18\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995F9822-2F1B-402F-B001-8832266C85E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97673E55-0506-43B9-BA69-F59EB144908D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="8544" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UC_CCS" sheetId="1" r:id="rId1"/>
@@ -67,10 +67,6 @@
     <t>ELCGAS</t>
   </si>
   <si>
-    <t>EPP*CCS*</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>ELCCO2N</t>
   </si>
   <si>
@@ -145,35 +141,34 @@
     <t>Maximum CCS capacity in the Kilroot area</t>
   </si>
   <si>
-    <t>EPP*Moneypoint*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EPP*Cork*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EPP*Dublin*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EPP*Offaly*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EPP*Kilroot*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>P-TH*CCS*</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>P-TH*Moneypoint*</t>
+  </si>
+  <si>
+    <t>P-TH*Cork*</t>
+  </si>
+  <si>
+    <t>P-TH*Dublin*</t>
+  </si>
+  <si>
+    <t>P-TH*Offaly*</t>
+  </si>
+  <si>
+    <t>P-TH*Kilroot*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -191,7 +186,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -594,13 +589,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +612,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -646,7 +644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="7" t="s">
@@ -660,17 +658,17 @@
         <v>12</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="9" t="s">
@@ -684,17 +682,17 @@
         <v>12</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="7" t="s">
@@ -705,20 +703,20 @@
         <v>11.795999999999999</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="7" t="s">
@@ -729,20 +727,20 @@
         <v>12.144</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="9" t="s">
@@ -753,20 +751,20 @@
         <v>87.204000000000008</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
@@ -777,42 +775,42 @@
         <v>95.855999999999995</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
+    </row>
+    <row r="12" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="B12" s="13" t="s">
+    <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="B13" s="13" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="E14" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="14" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="B15" s="14" t="s">
-        <v>22</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>7</v>
@@ -824,27 +822,27 @@
         <v>2</v>
       </c>
       <c r="F15" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="H15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="I15" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="14" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="B16" t="s">
-        <v>27</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -856,18 +854,18 @@
         <v>5</v>
       </c>
       <c r="I16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" t="s">
-        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -879,18 +877,18 @@
         <v>5</v>
       </c>
       <c r="I17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="B18" t="s">
-        <v>32</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -902,18 +900,18 @@
         <v>5</v>
       </c>
       <c r="I18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="B19" t="s">
-        <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -925,18 +923,18 @@
         <v>5</v>
       </c>
       <c r="I19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9">
-      <c r="B20" t="s">
-        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -948,7 +946,7 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust naming convention and clean-up
- merge ELC SubRES into a single file
- add extra files
- remove some files
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_CCS.xlsx
+++ b/SuppXLS/Scen_ELC_CCS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\I3p0_ELC_12TS_1REG_2020.11.18\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995F9822-2F1B-402F-B001-8832266C85E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97673E55-0506-43B9-BA69-F59EB144908D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="8544" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UC_CCS" sheetId="1" r:id="rId1"/>
@@ -67,10 +67,6 @@
     <t>ELCGAS</t>
   </si>
   <si>
-    <t>EPP*CCS*</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>ELCCO2N</t>
   </si>
   <si>
@@ -145,35 +141,34 @@
     <t>Maximum CCS capacity in the Kilroot area</t>
   </si>
   <si>
-    <t>EPP*Moneypoint*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EPP*Cork*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EPP*Dublin*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EPP*Offaly*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EPP*Kilroot*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>P-TH*CCS*</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>P-TH*Moneypoint*</t>
+  </si>
+  <si>
+    <t>P-TH*Cork*</t>
+  </si>
+  <si>
+    <t>P-TH*Dublin*</t>
+  </si>
+  <si>
+    <t>P-TH*Offaly*</t>
+  </si>
+  <si>
+    <t>P-TH*Kilroot*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -191,7 +186,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -594,13 +589,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +612,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -646,7 +644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="7" t="s">
@@ -660,17 +658,17 @@
         <v>12</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="9" t="s">
@@ -684,17 +682,17 @@
         <v>12</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="7" t="s">
@@ -705,20 +703,20 @@
         <v>11.795999999999999</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="7" t="s">
@@ -729,20 +727,20 @@
         <v>12.144</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="9" t="s">
@@ -753,20 +751,20 @@
         <v>87.204000000000008</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
@@ -777,42 +775,42 @@
         <v>95.855999999999995</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
+    </row>
+    <row r="12" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="B12" s="13" t="s">
+    <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
-      <c r="B13" s="13" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="E14" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="14" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="B15" s="14" t="s">
-        <v>22</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>7</v>
@@ -824,27 +822,27 @@
         <v>2</v>
       </c>
       <c r="F15" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="H15" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="I15" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="14" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="B16" t="s">
-        <v>27</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -856,18 +854,18 @@
         <v>5</v>
       </c>
       <c r="I16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" t="s">
-        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -879,18 +877,18 @@
         <v>5</v>
       </c>
       <c r="I17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="B18" t="s">
-        <v>32</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -902,18 +900,18 @@
         <v>5</v>
       </c>
       <c r="I18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="B19" t="s">
-        <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -925,18 +923,18 @@
         <v>5</v>
       </c>
       <c r="I19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9">
-      <c r="B20" t="s">
-        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -948,7 +946,7 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extend constraints to the multi regional version and clean-up
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_CCS.xlsx
+++ b/SuppXLS/Scen_ELC_CCS.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530F52E3-2CE7-4817-AEEE-00D107DBC211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EBB6D4-5ACF-4BAB-868E-B253C6309114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="2" r:id="rId1"/>
     <sheet name="UC_CCS" sheetId="1" r:id="rId2"/>
     <sheet name="FLO_EMIS" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
@@ -499,7 +496,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,10 +529,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -708,9 +701,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -743,35 +735,34 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{55987F76-5838-41FD-B788-B326C3492F8D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -883,7 +874,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3DF24D6-507C-432D-8ACF-ECF6768B46A7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -919,59 +910,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Intro"/>
-      <sheetName val="Regions"/>
-      <sheetName val="RES"/>
-      <sheetName val="SETUP"/>
-      <sheetName val="EnergyBalance"/>
-      <sheetName val="RSD_Balance"/>
-      <sheetName val="Fuel-Age_Adj"/>
-      <sheetName val="COMM"/>
-      <sheetName val="EMIS"/>
-      <sheetName val="DIST"/>
-      <sheetName val="Sector_Fuels"/>
-      <sheetName val="Heating Drivers"/>
-      <sheetName val="Non-Heat Drivers"/>
-      <sheetName val="DwellingStocks"/>
-      <sheetName val="SHWLP-Apt"/>
-      <sheetName val="SHWLP-Att"/>
-      <sheetName val="SHWLP-Det"/>
-      <sheetName val="ApartmentEnergyData"/>
-      <sheetName val="AttachedEnergyData"/>
-      <sheetName val="DettachedEnergyData"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1295,13 +1233,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F071441-2996-400B-948C-BB555D1B8F18}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" style="18" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="18" customWidth="1"/>
@@ -1333,7 +1272,7 @@
     <col min="31" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C3" s="19" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -1447,12 +1386,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>57</v>
       </c>
@@ -1567,7 +1506,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>60</v>
       </c>
@@ -1684,7 +1623,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>61</v>
       </c>
@@ -1809,7 +1748,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>64</v>
       </c>
@@ -1817,7 +1756,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>66</v>
       </c>
@@ -1825,7 +1764,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>68</v>
       </c>
@@ -1833,7 +1772,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>70</v>
       </c>
@@ -1841,7 +1780,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>72</v>
       </c>
@@ -1849,7 +1788,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>74</v>
       </c>
@@ -1857,7 +1796,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>76</v>
       </c>
@@ -1865,7 +1804,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>78</v>
       </c>
@@ -1873,7 +1812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>80</v>
       </c>
@@ -1881,7 +1820,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>82</v>
       </c>
@@ -1889,7 +1828,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>84</v>
       </c>
@@ -1897,7 +1836,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>86</v>
       </c>
@@ -1905,7 +1844,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>88</v>
       </c>
@@ -1913,7 +1852,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>90</v>
       </c>
@@ -1921,7 +1860,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>92</v>
       </c>
@@ -1929,7 +1868,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>94</v>
       </c>
@@ -1937,7 +1876,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>96</v>
       </c>
@@ -1945,7 +1884,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>98</v>
       </c>
@@ -1953,7 +1892,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>100</v>
       </c>
@@ -1961,7 +1900,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>102</v>
       </c>
@@ -1969,7 +1908,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
         <v>104</v>
       </c>
@@ -1977,7 +1916,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>106</v>
       </c>
@@ -1985,7 +1924,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
         <v>108</v>
       </c>
@@ -1993,7 +1932,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>110</v>
       </c>
@@ -2001,7 +1940,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>112</v>
       </c>
@@ -2009,7 +1948,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>114</v>
       </c>
@@ -2017,7 +1956,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>116</v>
       </c>
@@ -2471,6 +2410,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0058FA53-D765-4D61-875F-79F603B8624E}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2664,6 +2604,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327522a6d5518d67d5f1063e9cc64cf0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ffd5532d255be23b9fb13183c07e1fd0" ns2:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -2809,22 +2764,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5B0C690-3E0C-4B9D-864A-3F51F2CB2C74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04886123-9BA9-4DD3-969B-04E608718995}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA27B0CF-89B5-4B4C-B311-C0E79941CE35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2840,21 +2797,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04886123-9BA9-4DD3-969B-04E608718995}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5B0C690-3E0C-4B9D-864A-3F51F2CB2C74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated hourly power sector model. Various improvements to accelerate runtime on conventional computer with ~32GB RAM inlcuding; - Myopic scenarios - 5 Period definitions to reduce memory and compute load - restart scenario cases from P5 base case -rapidly accelerates solution time. - Introduce carbon budgets for testing in conjunction with linear emission reduction
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_ELC_CCS.xlsx
+++ b/SuppXLS/Scen_ELC_CCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\I3p0_ELC_8760TS_1REG_2020.12.2\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\I3p0_ELC_12TS_1REG_2020.11.18\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C727C01-56D2-43F7-8947-EAE8E9807A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97673E55-0506-43B9-BA69-F59EB144908D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="2800" windowWidth="25800" windowHeight="10100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="8544" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UC_CCS" sheetId="1" r:id="rId1"/>
@@ -145,6 +145,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>P-TH*Moneypoint*</t>
+  </si>
+  <si>
     <t>P-TH*Cork*</t>
   </si>
   <si>
@@ -155,10 +158,6 @@
   </si>
   <si>
     <t>P-TH*Kilroot*</t>
-  </si>
-  <si>
-    <t>P-TH*MP*</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -591,7 +590,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C16" sqref="C16:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -840,7 +839,7 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
         <v>27</v>
@@ -863,7 +862,7 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
         <v>27</v>
@@ -886,7 +885,7 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
         <v>27</v>
@@ -909,7 +908,7 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
         <v>27</v>
@@ -932,7 +931,7 @@
         <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>

</xml_diff>